<commit_message>
Overview te sluiten projecten gefinaliseerd
</commit_message>
<xml_diff>
--- a/Output/Werkbestand_AlleProjecten_2025-10-30.xlsx
+++ b/Output/Werkbestand_AlleProjecten_2025-10-30.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bram.gerrits\Desktop\Automations\ProjectAdministration\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{334D5065-E1A2-4B74-800B-80574E4A3FD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B613808-AF2E-4FEE-9A4F-2605F0DB38DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$N$2160</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$2:$E$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$2:$G$32</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11647" uniqueCount="4473">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11657" uniqueCount="4477">
   <si>
     <t>Datum: 2025-10-30</t>
   </si>
@@ -13471,6 +13471,18 @@
   </si>
   <si>
     <t>Projectnummer</t>
+  </si>
+  <si>
+    <t>Eindacties</t>
+  </si>
+  <si>
+    <t>Finale check</t>
+  </si>
+  <si>
+    <t>Gesloten SO met openstaande bestelling</t>
+  </si>
+  <si>
+    <t>Gesloten SO met openstaande PO - Proto</t>
   </si>
   <si>
     <t>Quote--31148613-2</t>
@@ -13514,7 +13526,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -13543,6 +13555,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF4F81BD"/>
         <bgColor rgb="FF4F81BD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFD7B5"/>
+        <bgColor rgb="FFFFD7B5"/>
       </patternFill>
     </fill>
   </fills>
@@ -13582,7 +13606,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -13621,11 +13645,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -13903,9 +13950,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N2160"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A939" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D942" sqref="D942"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13957,19 +14004,19 @@
       <c r="E2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="5" t="s">
         <v>8</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="5" t="s">
         <v>10</v>
       </c>
       <c r="K2" s="5" t="s">
@@ -80105,24 +80152,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.88671875" customWidth="1"/>
-    <col min="5" max="5" width="36" bestFit="1" customWidth="1"/>
-    <col min="6" max="10" width="17.77734375" customWidth="1"/>
+    <col min="1" max="4" width="17.77734375" customWidth="1"/>
+    <col min="5" max="6" width="35.77734375" customWidth="1"/>
+    <col min="7" max="10" width="17.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4468</v>
       </c>
@@ -80133,8 +80177,10 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>4469</v>
       </c>
@@ -80150,8 +80196,14 @@
       <c r="E2" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F2" s="2" t="s">
+        <v>4470</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>4471</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>126</v>
       </c>
@@ -80167,8 +80219,10 @@
       <c r="E3" s="15" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F3" s="15"/>
+      <c r="G3" s="16"/>
+    </row>
+    <row r="4" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
         <v>136</v>
       </c>
@@ -80184,231 +80238,259 @@
       <c r="E4" s="15" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F4" s="15"/>
+      <c r="G4" s="16"/>
+    </row>
+    <row r="5" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
-        <v>152</v>
+        <v>171</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>16</v>
+        <v>172</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>78</v>
+        <v>173</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>153</v>
+        <v>174</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+        <v>175</v>
+      </c>
+      <c r="F5" s="15"/>
+      <c r="G5" s="16"/>
+    </row>
+    <row r="6" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
-        <v>156</v>
+        <v>1037</v>
       </c>
       <c r="B6" s="15" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>17</v>
+        <v>85</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>157</v>
+        <v>1038</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+      <c r="F6" s="15"/>
+      <c r="G6" s="16"/>
+    </row>
+    <row r="7" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
-        <v>171</v>
+        <v>1548</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>172</v>
+        <v>16</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>173</v>
+        <v>53</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>174</v>
+        <v>1549</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1547</v>
+      </c>
+      <c r="F7" s="15"/>
+      <c r="G7" s="16"/>
+    </row>
+    <row r="8" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
-        <v>1037</v>
+        <v>1553</v>
       </c>
       <c r="B8" s="15" t="s">
         <v>16</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>1038</v>
+        <v>1554</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1555</v>
+      </c>
+      <c r="F8" s="15"/>
+      <c r="G8" s="16"/>
+    </row>
+    <row r="9" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
-        <v>1545</v>
+        <v>1866</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>16</v>
+        <v>172</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>53</v>
+        <v>121</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>1546</v>
+        <v>1867</v>
       </c>
       <c r="E9" s="15" t="s">
         <v>1547</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F9" s="15"/>
+      <c r="G9" s="16"/>
+    </row>
+    <row r="10" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
-        <v>1548</v>
+        <v>1868</v>
       </c>
       <c r="B10" s="15" t="s">
         <v>16</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>1549</v>
+        <v>1869</v>
       </c>
       <c r="E10" s="15" t="s">
         <v>1547</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F10" s="15"/>
+      <c r="G10" s="16"/>
+    </row>
+    <row r="11" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
-        <v>1553</v>
+        <v>1913</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>16</v>
+        <v>172</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>53</v>
+        <v>121</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>1554</v>
+        <v>1914</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>1555</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+        <v>4475</v>
+      </c>
+      <c r="F11" s="15"/>
+      <c r="G11" s="16"/>
+    </row>
+    <row r="12" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
-        <v>1687</v>
+        <v>2105</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>16</v>
+        <v>1655</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>36</v>
+        <v>1656</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>1688</v>
+        <v>2106</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>1689</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+        <v>2108</v>
+      </c>
+      <c r="F12" s="15"/>
+      <c r="G12" s="16"/>
+    </row>
+    <row r="13" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
-        <v>1830</v>
+        <v>2127</v>
       </c>
       <c r="B13" s="15" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>4470</v>
+        <v>106</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>1832</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1547</v>
+      </c>
+      <c r="F13" s="15"/>
+      <c r="G13" s="16"/>
+    </row>
+    <row r="14" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
-        <v>1866</v>
+        <v>2384</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>172</v>
+        <v>16</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>121</v>
+        <v>2148</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>1867</v>
+        <v>2385</v>
       </c>
       <c r="E14" s="15" t="s">
         <v>1547</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F14" s="15"/>
+      <c r="G14" s="16"/>
+    </row>
+    <row r="15" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
-        <v>1868</v>
+        <v>2669</v>
       </c>
       <c r="B15" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>2670</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>4476</v>
+      </c>
+      <c r="F15" s="15"/>
+      <c r="G15" s="16"/>
+    </row>
+    <row r="16" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="15" t="s">
+        <v>2682</v>
+      </c>
+      <c r="B16" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>1869</v>
-      </c>
-      <c r="E15" s="15" t="s">
+      <c r="C16" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>2683</v>
+      </c>
+      <c r="E16" s="15" t="s">
         <v>1547</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="15" t="s">
-        <v>1913</v>
-      </c>
-      <c r="B16" s="15" t="s">
-        <v>172</v>
-      </c>
-      <c r="C16" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="D16" s="15" t="s">
-        <v>1914</v>
-      </c>
-      <c r="E16" s="15" t="s">
-        <v>4471</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F16" s="15"/>
+      <c r="G16" s="16"/>
+    </row>
+    <row r="17" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
-        <v>2105</v>
+        <v>2800</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>1655</v>
+        <v>16</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>1656</v>
+        <v>85</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>2106</v>
+        <v>2801</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>2108</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1547</v>
+      </c>
+      <c r="F17" s="15"/>
+      <c r="G17" s="16"/>
+    </row>
+    <row r="18" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="s">
-        <v>2127</v>
+        <v>2810</v>
       </c>
       <c r="B18" s="15" t="s">
         <v>16</v>
@@ -80417,236 +80499,278 @@
         <v>85</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E18" s="15" t="s">
         <v>1547</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F18" s="15"/>
+      <c r="G18" s="16"/>
+    </row>
+    <row r="19" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="15" t="s">
-        <v>2147</v>
+        <v>3005</v>
       </c>
       <c r="B19" s="15" t="s">
         <v>16</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>2148</v>
+        <v>85</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>2149</v>
+        <v>106</v>
       </c>
       <c r="E19" s="15" t="s">
         <v>1547</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F19" s="15"/>
+      <c r="G19" s="16"/>
+    </row>
+    <row r="20" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="15" t="s">
-        <v>2235</v>
+        <v>3074</v>
       </c>
       <c r="B20" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>2148</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>3075</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>1547</v>
+      </c>
+      <c r="F20" s="15"/>
+      <c r="G20" s="16"/>
+    </row>
+    <row r="21" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="15" t="s">
+        <v>3242</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>3243</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>3244</v>
+      </c>
+      <c r="F21" s="15"/>
+      <c r="G21" s="16"/>
+    </row>
+    <row r="22" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="15" t="s">
+        <v>3245</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>3243</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>3244</v>
+      </c>
+      <c r="F22" s="15"/>
+      <c r="G22" s="16"/>
+    </row>
+    <row r="23" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="15" t="s">
+        <v>3246</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>3243</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>3244</v>
+      </c>
+      <c r="F23" s="15"/>
+      <c r="G23" s="16"/>
+    </row>
+    <row r="24" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="15" t="s">
+        <v>3521</v>
+      </c>
+      <c r="B24" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="15" t="s">
+      <c r="C24" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="D20" s="15" t="s">
-        <v>2236</v>
-      </c>
-      <c r="E20" s="15" t="s">
-        <v>2237</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="15" t="s">
-        <v>2384</v>
-      </c>
-      <c r="B21" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C21" s="15" t="s">
-        <v>2148</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>2385</v>
-      </c>
-      <c r="E21" s="15" t="s">
-        <v>1547</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="15" t="s">
-        <v>2422</v>
-      </c>
-      <c r="B22" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="D22" s="15" t="s">
-        <v>2423</v>
-      </c>
-      <c r="E22" s="15" t="s">
-        <v>2424</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="15" t="s">
-        <v>2669</v>
-      </c>
-      <c r="B23" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C23" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="D23" s="15" t="s">
-        <v>2670</v>
-      </c>
-      <c r="E23" s="15" t="s">
-        <v>4472</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="15" t="s">
-        <v>2682</v>
-      </c>
-      <c r="B24" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C24" s="15" t="s">
-        <v>85</v>
-      </c>
       <c r="D24" s="15" t="s">
-        <v>2683</v>
+        <v>3522</v>
       </c>
       <c r="E24" s="15" t="s">
-        <v>1547</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+        <v>3523</v>
+      </c>
+      <c r="F24" s="15"/>
+      <c r="G24" s="16"/>
+    </row>
+    <row r="25" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="15" t="s">
-        <v>2800</v>
+        <v>152</v>
       </c>
       <c r="B25" s="15" t="s">
         <v>16</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>2801</v>
+        <v>153</v>
       </c>
       <c r="E25" s="15" t="s">
-        <v>1547</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+      <c r="F25" s="15" t="s">
+        <v>4472</v>
+      </c>
+      <c r="G25" s="17"/>
+    </row>
+    <row r="26" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="15" t="s">
-        <v>2810</v>
+        <v>156</v>
       </c>
       <c r="B26" s="15" t="s">
         <v>16</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>85</v>
+        <v>17</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>104</v>
+        <v>157</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>1547</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+      <c r="F26" s="15" t="s">
+        <v>4473</v>
+      </c>
+      <c r="G26" s="17"/>
+    </row>
+    <row r="27" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="15" t="s">
-        <v>3005</v>
+        <v>1545</v>
       </c>
       <c r="B27" s="15" t="s">
         <v>16</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>106</v>
+        <v>1546</v>
       </c>
       <c r="E27" s="15" t="s">
         <v>1547</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F27" s="15" t="s">
+        <v>4473</v>
+      </c>
+      <c r="G27" s="17"/>
+    </row>
+    <row r="28" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="15" t="s">
-        <v>3074</v>
+        <v>1687</v>
       </c>
       <c r="B28" s="15" t="s">
         <v>16</v>
       </c>
       <c r="C28" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>1688</v>
+      </c>
+      <c r="E28" s="15" t="s">
+        <v>1689</v>
+      </c>
+      <c r="F28" s="15" t="s">
+        <v>4472</v>
+      </c>
+      <c r="G28" s="17"/>
+    </row>
+    <row r="29" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="15" t="s">
+        <v>1830</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>4474</v>
+      </c>
+      <c r="E29" s="15" t="s">
+        <v>1832</v>
+      </c>
+      <c r="F29" s="15" t="s">
+        <v>4473</v>
+      </c>
+      <c r="G29" s="17"/>
+    </row>
+    <row r="30" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="15" t="s">
+        <v>2147</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C30" s="15" t="s">
         <v>2148</v>
       </c>
-      <c r="D28" s="15" t="s">
-        <v>3075</v>
-      </c>
-      <c r="E28" s="15" t="s">
+      <c r="D30" s="15" t="s">
+        <v>2149</v>
+      </c>
+      <c r="E30" s="15" t="s">
         <v>1547</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="15" t="s">
-        <v>3242</v>
-      </c>
-      <c r="B29" s="15" t="s">
-        <v>172</v>
-      </c>
-      <c r="C29" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="D29" s="15" t="s">
-        <v>3243</v>
-      </c>
-      <c r="E29" s="15" t="s">
-        <v>3244</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="15" t="s">
-        <v>3245</v>
-      </c>
-      <c r="B30" s="15" t="s">
-        <v>172</v>
-      </c>
-      <c r="C30" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="D30" s="15" t="s">
-        <v>3243</v>
-      </c>
-      <c r="E30" s="15" t="s">
-        <v>3244</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F30" s="15" t="s">
+        <v>4473</v>
+      </c>
+      <c r="G30" s="17"/>
+    </row>
+    <row r="31" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="15" t="s">
-        <v>3246</v>
+        <v>2235</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>172</v>
+        <v>29</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>121</v>
+        <v>53</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>3243</v>
+        <v>2236</v>
       </c>
       <c r="E31" s="15" t="s">
-        <v>3244</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+        <v>2237</v>
+      </c>
+      <c r="F31" s="15" t="s">
+        <v>4473</v>
+      </c>
+      <c r="G31" s="17"/>
+    </row>
+    <row r="32" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="15" t="s">
-        <v>3521</v>
+        <v>2422</v>
       </c>
       <c r="B32" s="15" t="s">
         <v>29</v>
@@ -80655,14 +80779,22 @@
         <v>53</v>
       </c>
       <c r="D32" s="15" t="s">
-        <v>3522</v>
+        <v>2423</v>
       </c>
       <c r="E32" s="15" t="s">
-        <v>3523</v>
-      </c>
+        <v>2424</v>
+      </c>
+      <c r="F32" s="15" t="s">
+        <v>4473</v>
+      </c>
+      <c r="G32" s="17"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:E32" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <autoFilter ref="A2:G32" xr:uid="{00000000-0009-0000-0000-000001000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:G32">
+      <sortCondition sortBy="cellColor" ref="G2:G32" dxfId="1"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Sheet 3 aangemaakt binnen werkbestand. Deze gaat dienen als probleemfacturen overzicht. Op deze wijze kan ik beter aan de probleem facturen werken
</commit_message>
<xml_diff>
--- a/Output/Werkbestand_AlleProjecten_2025-10-30.xlsx
+++ b/Output/Werkbestand_AlleProjecten_2025-10-30.xlsx
@@ -8,17 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bram.gerrits\Desktop\Automations\ProjectAdministration\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B613808-AF2E-4FEE-9A4F-2605F0DB38DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C52D11A4-F263-457D-B844-B4EAD4504B23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$N$2160</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$2:$G$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Sheet3!$A$2:$E$39</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11657" uniqueCount="4477">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11846" uniqueCount="4481">
   <si>
     <t>Datum: 2025-10-30</t>
   </si>
@@ -13467,9 +13469,6 @@
     <t>RETOUREN 2025 VLD</t>
   </si>
   <si>
-    <t xml:space="preserve">Datum: </t>
-  </si>
-  <si>
     <t>Projectnummer</t>
   </si>
   <si>
@@ -13492,6 +13491,21 @@
   </si>
   <si>
     <t>Afsluiten nadat gefactureerd is.</t>
+  </si>
+  <si>
+    <t>Deze heeft een dochter project die open staat. Dit kunnen we niet in Sumatra zien. Inzichtelijk maken welke orderregels openstaan bij dochterproject.</t>
+  </si>
+  <si>
+    <t>Tjerk vragen om RAD.DH1.00010 Panel staat op -3. dit moet gecorrigeerd worden.</t>
+  </si>
+  <si>
+    <t>Hier worden uren factureerd. Contact opnemen met receptie</t>
+  </si>
+  <si>
+    <t>Er zijn uren gefactureerd. Hoe lossen we dit op?</t>
+  </si>
+  <si>
+    <t>Deze gaat nog Sandy</t>
   </si>
 </sst>
 </file>
@@ -13655,24 +13669,7 @@
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -13950,9 +13947,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N2160"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A939" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D942" sqref="D942"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -80155,8 +80152,8 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -80167,13 +80164,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>4468</v>
-      </c>
-      <c r="B1" s="1" t="str">
+      <c r="A1" s="1" t="str">
         <f ca="1">"Datum: "&amp;TEXT(NOW(),"dd-mm-jjjj")</f>
         <v>Datum: 30-10-2025</v>
       </c>
+      <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -80182,7 +80177,7 @@
     </row>
     <row r="2" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>4469</v>
+        <v>4468</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
@@ -80197,10 +80192,10 @@
         <v>10</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>4469</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>4470</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>4471</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -80243,111 +80238,117 @@
     </row>
     <row r="5" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
-        <v>171</v>
+        <v>152</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>172</v>
+        <v>16</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>173</v>
+        <v>78</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>174</v>
+        <v>153</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>175</v>
-      </c>
-      <c r="F5" s="15"/>
-      <c r="G5" s="16"/>
+        <v>130</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>4471</v>
+      </c>
+      <c r="G5" s="17"/>
     </row>
     <row r="6" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
-        <v>1037</v>
+        <v>156</v>
       </c>
       <c r="B6" s="15" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>85</v>
+        <v>17</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>1038</v>
+        <v>157</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>130</v>
-      </c>
-      <c r="F6" s="15"/>
-      <c r="G6" s="16"/>
+        <v>159</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>4472</v>
+      </c>
+      <c r="G6" s="17"/>
     </row>
     <row r="7" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
-        <v>1548</v>
+        <v>171</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>16</v>
+        <v>172</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>53</v>
+        <v>173</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>1549</v>
+        <v>174</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>1547</v>
+        <v>175</v>
       </c>
       <c r="F7" s="15"/>
       <c r="G7" s="16"/>
     </row>
     <row r="8" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
-        <v>1553</v>
+        <v>1037</v>
       </c>
       <c r="B8" s="15" t="s">
         <v>16</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>1554</v>
+        <v>1038</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>1555</v>
+        <v>130</v>
       </c>
       <c r="F8" s="15"/>
       <c r="G8" s="16"/>
     </row>
     <row r="9" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
-        <v>1866</v>
+        <v>1545</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>172</v>
+        <v>16</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>121</v>
+        <v>53</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>1867</v>
+        <v>1546</v>
       </c>
       <c r="E9" s="15" t="s">
         <v>1547</v>
       </c>
-      <c r="F9" s="15"/>
-      <c r="G9" s="16"/>
+      <c r="F9" s="15" t="s">
+        <v>4472</v>
+      </c>
+      <c r="G9" s="17"/>
     </row>
     <row r="10" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
-        <v>1868</v>
+        <v>1548</v>
       </c>
       <c r="B10" s="15" t="s">
         <v>16</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>1869</v>
+        <v>1549</v>
       </c>
       <c r="E10" s="15" t="s">
         <v>1547</v>
@@ -80357,444 +80358,1111 @@
     </row>
     <row r="11" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
+        <v>1553</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>1554</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>1555</v>
+      </c>
+      <c r="F11" s="15"/>
+      <c r="G11" s="16"/>
+    </row>
+    <row r="12" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="15" t="s">
+        <v>1687</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>1688</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>1689</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>4471</v>
+      </c>
+      <c r="G12" s="17"/>
+    </row>
+    <row r="13" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="15" t="s">
+        <v>1830</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>4473</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>1832</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>4472</v>
+      </c>
+      <c r="G13" s="17"/>
+    </row>
+    <row r="14" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="15" t="s">
+        <v>1866</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>1867</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>1547</v>
+      </c>
+      <c r="F14" s="15"/>
+      <c r="G14" s="16"/>
+    </row>
+    <row r="15" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="15" t="s">
+        <v>1868</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>1869</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>1547</v>
+      </c>
+      <c r="F15" s="15"/>
+      <c r="G15" s="16"/>
+    </row>
+    <row r="16" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="15" t="s">
         <v>1913</v>
       </c>
+      <c r="B16" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>1914</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>4474</v>
+      </c>
+      <c r="F16" s="15"/>
+      <c r="G16" s="16"/>
+    </row>
+    <row r="17" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="15" t="s">
+        <v>2105</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>1655</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>1656</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>2106</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>2108</v>
+      </c>
+      <c r="F17" s="15"/>
+      <c r="G17" s="16"/>
+    </row>
+    <row r="18" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="15" t="s">
+        <v>2127</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>1547</v>
+      </c>
+      <c r="F18" s="15"/>
+      <c r="G18" s="16"/>
+    </row>
+    <row r="19" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="15" t="s">
+        <v>2147</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>2148</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>2149</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>1547</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>4472</v>
+      </c>
+      <c r="G19" s="17"/>
+    </row>
+    <row r="20" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="15" t="s">
+        <v>2235</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>2236</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>2237</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>4472</v>
+      </c>
+      <c r="G20" s="17"/>
+    </row>
+    <row r="21" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="15" t="s">
+        <v>2384</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>2148</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>2385</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>1547</v>
+      </c>
+      <c r="F21" s="15"/>
+      <c r="G21" s="16"/>
+    </row>
+    <row r="22" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="15" t="s">
+        <v>2422</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>2423</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>2424</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>4472</v>
+      </c>
+      <c r="G22" s="17"/>
+    </row>
+    <row r="23" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="15" t="s">
+        <v>2669</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>2670</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>4475</v>
+      </c>
+      <c r="F23" s="15"/>
+      <c r="G23" s="16"/>
+    </row>
+    <row r="24" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="15" t="s">
+        <v>2682</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>2683</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>1547</v>
+      </c>
+      <c r="F24" s="15"/>
+      <c r="G24" s="16"/>
+    </row>
+    <row r="25" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="15" t="s">
+        <v>2800</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>2801</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>1547</v>
+      </c>
+      <c r="F25" s="15"/>
+      <c r="G25" s="16"/>
+    </row>
+    <row r="26" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="15" t="s">
+        <v>2810</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="E26" s="15" t="s">
+        <v>1547</v>
+      </c>
+      <c r="F26" s="15"/>
+      <c r="G26" s="16"/>
+    </row>
+    <row r="27" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="15" t="s">
+        <v>3005</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>1547</v>
+      </c>
+      <c r="F27" s="15"/>
+      <c r="G27" s="16"/>
+    </row>
+    <row r="28" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="15" t="s">
+        <v>3074</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>2148</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>3075</v>
+      </c>
+      <c r="E28" s="15" t="s">
+        <v>1547</v>
+      </c>
+      <c r="F28" s="15"/>
+      <c r="G28" s="16"/>
+    </row>
+    <row r="29" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="15" t="s">
+        <v>3242</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>3243</v>
+      </c>
+      <c r="E29" s="15" t="s">
+        <v>3244</v>
+      </c>
+      <c r="F29" s="15"/>
+      <c r="G29" s="16"/>
+    </row>
+    <row r="30" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="15" t="s">
+        <v>3245</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>3243</v>
+      </c>
+      <c r="E30" s="15" t="s">
+        <v>3244</v>
+      </c>
+      <c r="F30" s="15"/>
+      <c r="G30" s="16"/>
+    </row>
+    <row r="31" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="15" t="s">
+        <v>3246</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="D31" s="15" t="s">
+        <v>3243</v>
+      </c>
+      <c r="E31" s="15" t="s">
+        <v>3244</v>
+      </c>
+      <c r="F31" s="15"/>
+      <c r="G31" s="16"/>
+    </row>
+    <row r="32" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="15" t="s">
+        <v>3521</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D32" s="15" t="s">
+        <v>3522</v>
+      </c>
+      <c r="E32" s="15" t="s">
+        <v>3523</v>
+      </c>
+      <c r="F32" s="15"/>
+      <c r="G32" s="16"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A2:G32" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:E39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="4" width="17.77734375" customWidth="1"/>
+    <col min="5" max="5" width="40.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="str">
+        <f ca="1">"Datum: "&amp;TEXT(NOW(),"dd-mm-jjjj")</f>
+        <v>Datum: 30-10-2025</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>4468</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>4476</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>4477</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="15" t="s">
+        <v>1550</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>1551</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>1552</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="15" t="s">
+        <v>1617</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>1618</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="15" t="s">
+        <v>1620</v>
+      </c>
       <c r="B11" s="15" t="s">
-        <v>172</v>
+        <v>22</v>
       </c>
       <c r="C11" s="15" t="s">
         <v>121</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>1914</v>
+        <v>1621</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>4475</v>
-      </c>
-      <c r="F11" s="15"/>
-      <c r="G11" s="16"/>
-    </row>
-    <row r="12" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
-        <v>2105</v>
+        <v>2021</v>
       </c>
       <c r="B12" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>2022</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="15" t="s">
+        <v>2049</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>2050</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="15" t="s">
+        <v>2287</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>1980</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>2288</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>2289</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>2291</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="15" t="s">
+        <v>2578</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>2579</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>2580</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>2581</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="15" t="s">
+        <v>2668</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="15" t="s">
+        <v>2762</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>2763</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>1712</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>2764</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>2765</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="15" t="s">
+        <v>2914</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>2805</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>2915</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="15" t="s">
+        <v>2920</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>2921</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="15" t="s">
+        <v>3071</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>3072</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>4478</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="15" t="s">
+        <v>3076</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>3077</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="15" t="s">
+        <v>3080</v>
+      </c>
+      <c r="B22" s="15" t="s">
         <v>1655</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>1656</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>2106</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>2108</v>
-      </c>
-      <c r="F12" s="15"/>
-      <c r="G12" s="16"/>
-    </row>
-    <row r="13" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="15" t="s">
-        <v>2127</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>1547</v>
-      </c>
-      <c r="F13" s="15"/>
-      <c r="G13" s="16"/>
-    </row>
-    <row r="14" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="15" t="s">
-        <v>2384</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>2148</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>2385</v>
-      </c>
-      <c r="E14" s="15" t="s">
-        <v>1547</v>
-      </c>
-      <c r="F14" s="15"/>
-      <c r="G14" s="16"/>
-    </row>
-    <row r="15" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="15" t="s">
-        <v>2669</v>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>2670</v>
-      </c>
-      <c r="E15" s="15" t="s">
-        <v>4476</v>
-      </c>
-      <c r="F15" s="15"/>
-      <c r="G15" s="16"/>
-    </row>
-    <row r="16" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="15" t="s">
-        <v>2682</v>
-      </c>
-      <c r="B16" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="D16" s="15" t="s">
-        <v>2683</v>
-      </c>
-      <c r="E16" s="15" t="s">
-        <v>1547</v>
-      </c>
-      <c r="F16" s="15"/>
-      <c r="G16" s="16"/>
-    </row>
-    <row r="17" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="15" t="s">
-        <v>2800</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>2801</v>
-      </c>
-      <c r="E17" s="15" t="s">
-        <v>1547</v>
-      </c>
-      <c r="F17" s="15"/>
-      <c r="G17" s="16"/>
-    </row>
-    <row r="18" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="15" t="s">
-        <v>2810</v>
-      </c>
-      <c r="B18" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="E18" s="15" t="s">
-        <v>1547</v>
-      </c>
-      <c r="F18" s="15"/>
-      <c r="G18" s="16"/>
-    </row>
-    <row r="19" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="15" t="s">
-        <v>3005</v>
-      </c>
-      <c r="B19" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="D19" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="E19" s="15" t="s">
-        <v>1547</v>
-      </c>
-      <c r="F19" s="15"/>
-      <c r="G19" s="16"/>
-    </row>
-    <row r="20" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="15" t="s">
-        <v>3074</v>
-      </c>
-      <c r="B20" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20" s="15" t="s">
-        <v>2148</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>3075</v>
-      </c>
-      <c r="E20" s="15" t="s">
-        <v>1547</v>
-      </c>
-      <c r="F20" s="15"/>
-      <c r="G20" s="16"/>
-    </row>
-    <row r="21" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="15" t="s">
-        <v>3242</v>
-      </c>
-      <c r="B21" s="15" t="s">
-        <v>172</v>
-      </c>
-      <c r="C21" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>3243</v>
-      </c>
-      <c r="E21" s="15" t="s">
-        <v>3244</v>
-      </c>
-      <c r="F21" s="15"/>
-      <c r="G21" s="16"/>
-    </row>
-    <row r="22" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="15" t="s">
-        <v>3245</v>
-      </c>
-      <c r="B22" s="15" t="s">
-        <v>172</v>
       </c>
       <c r="C22" s="15" t="s">
         <v>121</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>3243</v>
+        <v>3081</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>3244</v>
-      </c>
-      <c r="F22" s="15"/>
-      <c r="G22" s="16"/>
-    </row>
-    <row r="23" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+        <v>3082</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="15" t="s">
-        <v>3246</v>
+        <v>3095</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>172</v>
+        <v>127</v>
       </c>
       <c r="C23" s="15" t="s">
         <v>121</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>3243</v>
+        <v>3096</v>
       </c>
       <c r="E23" s="15" t="s">
-        <v>3244</v>
-      </c>
-      <c r="F23" s="15"/>
-      <c r="G23" s="16"/>
-    </row>
-    <row r="24" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="15" t="s">
-        <v>3521</v>
+        <v>3113</v>
       </c>
       <c r="B24" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>3114</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="15" t="s">
+        <v>3199</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>3200</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>1981</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>3201</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>3202</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="15" t="s">
+        <v>3254</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>2805</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>3255</v>
+      </c>
+      <c r="E26" s="15" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="15" t="s">
+        <v>3305</v>
+      </c>
+      <c r="B27" s="15" t="s">
         <v>29</v>
-      </c>
-      <c r="C24" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="D24" s="15" t="s">
-        <v>3522</v>
-      </c>
-      <c r="E24" s="15" t="s">
-        <v>3523</v>
-      </c>
-      <c r="F24" s="15"/>
-      <c r="G24" s="16"/>
-    </row>
-    <row r="25" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="15" t="s">
-        <v>152</v>
-      </c>
-      <c r="B25" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C25" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="D25" s="15" t="s">
-        <v>153</v>
-      </c>
-      <c r="E25" s="15" t="s">
-        <v>130</v>
-      </c>
-      <c r="F25" s="15" t="s">
-        <v>4472</v>
-      </c>
-      <c r="G25" s="17"/>
-    </row>
-    <row r="26" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="15" t="s">
-        <v>156</v>
-      </c>
-      <c r="B26" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C26" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D26" s="15" t="s">
-        <v>157</v>
-      </c>
-      <c r="E26" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="F26" s="15" t="s">
-        <v>4473</v>
-      </c>
-      <c r="G26" s="17"/>
-    </row>
-    <row r="27" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="15" t="s">
-        <v>1545</v>
-      </c>
-      <c r="B27" s="15" t="s">
-        <v>16</v>
       </c>
       <c r="C27" s="15" t="s">
         <v>53</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>1546</v>
+        <v>3306</v>
       </c>
       <c r="E27" s="15" t="s">
-        <v>1547</v>
-      </c>
-      <c r="F27" s="15" t="s">
-        <v>4473</v>
-      </c>
-      <c r="G27" s="17"/>
-    </row>
-    <row r="28" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+        <v>3307</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="15" t="s">
-        <v>1687</v>
+        <v>3308</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>1688</v>
+        <v>3309</v>
       </c>
       <c r="E28" s="15" t="s">
-        <v>1689</v>
-      </c>
-      <c r="F28" s="15" t="s">
-        <v>4472</v>
-      </c>
-      <c r="G28" s="17"/>
-    </row>
-    <row r="29" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+        <v>4479</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="15" t="s">
-        <v>1830</v>
+        <v>3311</v>
       </c>
       <c r="B29" s="15" t="s">
         <v>16</v>
       </c>
       <c r="C29" s="15" t="s">
+        <v>651</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>3312</v>
+      </c>
+      <c r="E29" s="15" t="s">
+        <v>3313</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="15" t="s">
+        <v>3586</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>3587</v>
+      </c>
+      <c r="E30" s="15" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="15" t="s">
+        <v>3588</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>1655</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="D31" s="15" t="s">
+        <v>3589</v>
+      </c>
+      <c r="E31" s="15" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="15" t="s">
+        <v>3590</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>1655</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="D32" s="15" t="s">
+        <v>3591</v>
+      </c>
+      <c r="E32" s="15" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="15" t="s">
+        <v>3592</v>
+      </c>
+      <c r="B33" s="15" t="s">
+        <v>1655</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="D33" s="15" t="s">
+        <v>3593</v>
+      </c>
+      <c r="E33" s="15" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="15" t="s">
+        <v>3594</v>
+      </c>
+      <c r="B34" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C34" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="D29" s="15" t="s">
-        <v>4474</v>
-      </c>
-      <c r="E29" s="15" t="s">
-        <v>1832</v>
-      </c>
-      <c r="F29" s="15" t="s">
-        <v>4473</v>
-      </c>
-      <c r="G29" s="17"/>
-    </row>
-    <row r="30" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="15" t="s">
-        <v>2147</v>
-      </c>
-      <c r="B30" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C30" s="15" t="s">
-        <v>2148</v>
-      </c>
-      <c r="D30" s="15" t="s">
-        <v>2149</v>
-      </c>
-      <c r="E30" s="15" t="s">
-        <v>1547</v>
-      </c>
-      <c r="F30" s="15" t="s">
-        <v>4473</v>
-      </c>
-      <c r="G30" s="17"/>
-    </row>
-    <row r="31" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="15" t="s">
-        <v>2235</v>
-      </c>
-      <c r="B31" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C31" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="D31" s="15" t="s">
-        <v>2236</v>
-      </c>
-      <c r="E31" s="15" t="s">
-        <v>2237</v>
-      </c>
-      <c r="F31" s="15" t="s">
-        <v>4473</v>
-      </c>
-      <c r="G31" s="17"/>
-    </row>
-    <row r="32" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="15" t="s">
-        <v>2422</v>
-      </c>
-      <c r="B32" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C32" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="D32" s="15" t="s">
-        <v>2423</v>
-      </c>
-      <c r="E32" s="15" t="s">
-        <v>2424</v>
-      </c>
-      <c r="F32" s="15" t="s">
-        <v>4473</v>
-      </c>
-      <c r="G32" s="17"/>
+      <c r="D34" s="15" t="s">
+        <v>3595</v>
+      </c>
+      <c r="E34" s="15" t="s">
+        <v>4479</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="15" t="s">
+        <v>3624</v>
+      </c>
+      <c r="B35" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="D35" s="15" t="s">
+        <v>3625</v>
+      </c>
+      <c r="E35" s="15" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="15" t="s">
+        <v>3682</v>
+      </c>
+      <c r="B36" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="D36" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="E36" s="15" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="15" t="s">
+        <v>3741</v>
+      </c>
+      <c r="B37" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="D37" s="15" t="s">
+        <v>3742</v>
+      </c>
+      <c r="E37" s="15" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="15" t="s">
+        <v>3753</v>
+      </c>
+      <c r="B38" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="C38" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="D38" s="15" t="s">
+        <v>3754</v>
+      </c>
+      <c r="E38" s="15" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="15" t="s">
+        <v>3851</v>
+      </c>
+      <c r="B39" s="15" t="s">
+        <v>2176</v>
+      </c>
+      <c r="C39" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D39" s="15" t="s">
+        <v>3852</v>
+      </c>
+      <c r="E39" s="15" t="s">
+        <v>4480</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:G32" xr:uid="{00000000-0009-0000-0000-000001000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:G32">
-      <sortCondition sortBy="cellColor" ref="G2:G32" dxfId="1"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A2:E39" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>